<commit_message>
translate matrix 5x5 iso27005 in French
</commit_message>
<xml_diff>
--- a/tools/matrix/5x5-iso-27005/risk-matrix-5x5-iso-27005.xlsx
+++ b/tools/matrix/5x5-iso-27005/risk-matrix-5x5-iso-27005.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/matrix/5x5-iso-27005/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4499C39B-BA20-2C4B-B754-E17830FAB2A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43F6097-A6A7-7F48-9E11-3AB5390E0A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20480" activeTab="1" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="20300" activeTab="1" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="107">
   <si>
     <t>library_urn</t>
   </si>
@@ -201,9 +201,6 @@
     <t>5 - very high</t>
   </si>
   <si>
-    <t>5 - Catastrophic</t>
-  </si>
-  <si>
     <t>4 - critical</t>
   </si>
   <si>
@@ -244,6 +241,123 @@
   </si>
   <si>
     <t>very high - unacceptable risk</t>
+  </si>
+  <si>
+    <t>library_name[fr]</t>
+  </si>
+  <si>
+    <t>library_description[fr]</t>
+  </si>
+  <si>
+    <t>risk_matrix_name[fr]</t>
+  </si>
+  <si>
+    <t>risk_matrix_description[fr]</t>
+  </si>
+  <si>
+    <t>Matrice 5x5 ISO-27005</t>
+  </si>
+  <si>
+    <t>Matrice 5x5 décrite dans la norme ISO-27005 annexe A</t>
+  </si>
+  <si>
+    <t>name[fr]</t>
+  </si>
+  <si>
+    <t>description[fr]</t>
+  </si>
+  <si>
+    <t>5 - presque certain</t>
+  </si>
+  <si>
+    <t>4 - très probable</t>
+  </si>
+  <si>
+    <t>3 - probable</t>
+  </si>
+  <si>
+    <t>1 - peu probable</t>
+  </si>
+  <si>
+    <t>1 - mineur</t>
+  </si>
+  <si>
+    <t>2 - significatif</t>
+  </si>
+  <si>
+    <t>3 - serieux</t>
+  </si>
+  <si>
+    <t>4 - critique</t>
+  </si>
+  <si>
+    <t>5 - catastrophique</t>
+  </si>
+  <si>
+    <t>5 - catastrophic</t>
+  </si>
+  <si>
+    <t>1 - très faible</t>
+  </si>
+  <si>
+    <t>2 - faible</t>
+  </si>
+  <si>
+    <t>3 - moyen</t>
+  </si>
+  <si>
+    <t>4 - élevé</t>
+  </si>
+  <si>
+    <t>5 - très élevé</t>
+  </si>
+  <si>
+    <t>très faible - risque acceptable</t>
+  </si>
+  <si>
+    <t>faible - risque acceptable</t>
+  </si>
+  <si>
+    <t>moyen - risque tolerable</t>
+  </si>
+  <si>
+    <t>élevé - risque inacceptable</t>
+  </si>
+  <si>
+    <t>très élevé - risque inacceptable</t>
+  </si>
+  <si>
+    <t>Conséquences négligeables pour l'oraganisation</t>
+  </si>
+  <si>
+    <t>Conséquences significatives mais limitées pour l'organisation</t>
+  </si>
+  <si>
+    <t>Conséquences substantielles pour l'organisation</t>
+  </si>
+  <si>
+    <t>Conséquences désastreuses pour l'organisation</t>
+  </si>
+  <si>
+    <t>Conséquences sectorielles ou réglementaires au-delà de l’organisation</t>
+  </si>
+  <si>
+    <t>La vraisemblance du scénario de risque est très élevée</t>
+  </si>
+  <si>
+    <t>La vraisemblance du scénario de risque est élevée</t>
+  </si>
+  <si>
+    <t>La vraisemblance du scénario de risque est significative</t>
+  </si>
+  <si>
+    <t>2 - plutôt probable</t>
+  </si>
+  <si>
+    <t>La vraisemblance du scénario de risque est faible</t>
+  </si>
+  <si>
+    <t>La vraisemblance du scénario de risque est très faible</t>
   </si>
 </sst>
 </file>
@@ -387,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -426,31 +540,28 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -798,15 +909,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF47FB7-BAFE-4E46-A187-08E7F45C581C}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="177" workbookViewId="0">
+    <sheetView zoomScale="177" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="111.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -824,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -924,6 +1035,38 @@
       </c>
       <c r="C14" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -934,10 +1077,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C78439-E0E8-6B46-8D3C-6DE0FA8D6D39}">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="178" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,9 +1091,11 @@
     <col min="5" max="5" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="10.83203125" style="2"/>
+    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="49.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -984,8 +1129,14 @@
       <c r="K1" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -996,7 +1147,7 @@
         <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
         <v>28</v>
@@ -1010,14 +1161,20 @@
       <c r="I2" s="14">
         <v>3</v>
       </c>
-      <c r="J2" s="21">
+      <c r="J2" s="20">
         <v>4</v>
       </c>
-      <c r="K2" s="21">
+      <c r="K2" s="20">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="M2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1028,7 +1185,7 @@
         <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F3" t="s">
         <v>29</v>
@@ -1042,14 +1199,20 @@
       <c r="I3" s="15">
         <v>3</v>
       </c>
-      <c r="J3" s="22">
+      <c r="J3" s="21">
         <v>3</v>
       </c>
-      <c r="K3" s="21">
+      <c r="K3" s="20">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1060,7 +1223,7 @@
         <v>40</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4" t="s">
         <v>30</v>
@@ -1080,8 +1243,14 @@
       <c r="K4" s="16">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -1092,18 +1261,18 @@
         <v>39</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F5" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="18">
+      <c r="G5" s="13">
         <v>0</v>
       </c>
-      <c r="H5" s="19">
+      <c r="H5" s="18">
         <v>1</v>
       </c>
-      <c r="I5" s="19">
+      <c r="I5" s="18">
         <v>1</v>
       </c>
       <c r="J5" s="3">
@@ -1112,8 +1281,14 @@
       <c r="K5" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1124,28 +1299,34 @@
         <v>38</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="18">
+      <c r="G6" s="13">
         <v>0</v>
       </c>
-      <c r="H6" s="18">
+      <c r="H6" s="13">
         <v>0</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I6" s="19">
         <v>1</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="19">
         <v>1</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="19">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -1156,13 +1337,19 @@
         <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1173,13 +1360,19 @@
         <v>39</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="M8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1190,13 +1383,19 @@
         <v>40</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -1207,13 +1406,19 @@
         <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L10" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="M10" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1224,13 +1429,19 @@
         <v>42</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1245,10 +1456,16 @@
         <v>49</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1263,10 +1480,16 @@
         <v>50</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="L13" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -1281,10 +1504,16 @@
         <v>51</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1299,10 +1528,16 @@
         <v>52</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1317,7 +1552,13 @@
         <v>53</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix error in matrix
Thanks to geekbog detection
</commit_message>
<xml_diff>
--- a/tools/matrix/5x5-iso-27005/risk-matrix-5x5-iso-27005.xlsx
+++ b/tools/matrix/5x5-iso-27005/risk-matrix-5x5-iso-27005.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/matrix/5x5-iso-27005/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43F6097-A6A7-7F48-9E11-3AB5390E0A5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBF979C-2E92-7E4A-9AF0-569BCAE4094C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="20300" activeTab="1" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
     <sheet name="spec" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C78439-E0E8-6B46-8D3C-6DE0FA8D6D39}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="178" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1190,8 +1190,8 @@
       <c r="F3" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="3">
-        <v>2</v>
+      <c r="G3" s="17">
+        <v>1</v>
       </c>
       <c r="H3" s="3">
         <v>2</v>

</xml_diff>

<commit_message>
fix French translation for iso27005 matrix
</commit_message>
<xml_diff>
--- a/tools/matrix/5x5-iso-27005/risk-matrix-5x5-iso-27005.xlsx
+++ b/tools/matrix/5x5-iso-27005/risk-matrix-5x5-iso-27005.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericlaubacher/Documents/GitHub/ciso-assistant-community/tools/matrix/5x5-iso-27005/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBF979C-2E92-7E4A-9AF0-569BCAE4094C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB147526-EDEF-B845-8D10-0693FF792B75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="20300" activeTab="1" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34560" windowHeight="20300" xr2:uid="{737B4EAE-987D-4047-A963-C4AA7BEFCFC2}"/>
   </bookViews>
   <sheets>
     <sheet name="library_content" sheetId="1" r:id="rId1"/>
     <sheet name="spec" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -276,9 +276,6 @@
     <t>3 - probable</t>
   </si>
   <si>
-    <t>1 - peu probable</t>
-  </si>
-  <si>
     <t>1 - mineur</t>
   </si>
   <si>
@@ -351,13 +348,16 @@
     <t>La vraisemblance du scénario de risque est significative</t>
   </si>
   <si>
-    <t>2 - plutôt probable</t>
-  </si>
-  <si>
     <t>La vraisemblance du scénario de risque est faible</t>
   </si>
   <si>
     <t>La vraisemblance du scénario de risque est très faible</t>
+  </si>
+  <si>
+    <t>2 - plutôt improbable</t>
+  </si>
+  <si>
+    <t>1 - improbable</t>
   </si>
 </sst>
 </file>
@@ -911,8 +911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF47FB7-BAFE-4E46-A187-08E7F45C581C}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView zoomScale="177" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" zoomScale="177" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,7 +935,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1079,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C78439-E0E8-6B46-8D3C-6DE0FA8D6D39}">
   <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView topLeftCell="F1" zoomScale="178" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1091,7 +1091,7 @@
     <col min="5" max="5" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="10.83203125" style="2"/>
-    <col min="12" max="12" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="49.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1171,7 +1171,7 @@
         <v>76</v>
       </c>
       <c r="M2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1209,7 +1209,7 @@
         <v>77</v>
       </c>
       <c r="M3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -1247,7 +1247,7 @@
         <v>78</v>
       </c>
       <c r="M4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -1282,10 +1282,10 @@
         <v>2</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="M5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -1320,10 +1320,10 @@
         <v>1</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>79</v>
+        <v>106</v>
       </c>
       <c r="M6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -1343,10 +1343,10 @@
         <v>37</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -1366,10 +1366,10 @@
         <v>36</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -1389,10 +1389,10 @@
         <v>35</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -1412,10 +1412,10 @@
         <v>34</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -1429,16 +1429,16 @@
         <v>42</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F11" t="s">
         <v>33</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="M11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -1459,10 +1459,10 @@
         <v>63</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="M12" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -1483,10 +1483,10 @@
         <v>64</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -1507,10 +1507,10 @@
         <v>65</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -1531,10 +1531,10 @@
         <v>66</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1555,10 +1555,10 @@
         <v>67</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>